<commit_message>
Added backend communication (not tested).  Added Select Compartment size functionality in Admin and UI.  Added Test mode for testing w/o backend functioning.
</commit_message>
<xml_diff>
--- a/SmartLockerKiosk/DataDefinitions.xlsx
+++ b/SmartLockerKiosk/DataDefinitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SmartLockerA\SmartLockerKiosk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7DAA6D49-C5BF-4E5E-AA7F-964345F39AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95699A8-BEA1-43ED-B298-BD8FCF8730BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11385" yWindow="1020" windowWidth="38700" windowHeight="15345" xr2:uid="{BB9DCED8-1A07-458A-B8E4-0C59FD1F8135}"/>
+    <workbookView xWindow="29835" yWindow="5745" windowWidth="16650" windowHeight="15135" xr2:uid="{BB9DCED8-1A07-458A-B8E4-0C59FD1F8135}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>